<commit_message>
Añadido editor de datos
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
   <si>
     <t>game_title</t>
   </si>
@@ -25,6 +25,9 @@
     <t>name</t>
   </si>
   <si>
+    <t>url</t>
+  </si>
+  <si>
     <t>3D Grand Prix</t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t>Mad Mix Game</t>
   </si>
   <si>
+    <t>Navy Moves</t>
+  </si>
+  <si>
     <t>Oh Mummy</t>
   </si>
   <si>
@@ -320,13 +326,16 @@
   </si>
   <si>
     <t>Imagine</t>
+  </si>
+  <si>
+    <t>https://amstrad.es/doku.php?id=juegos:la_abadia_del_crimen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +350,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,16 +391,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,13 +699,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,778 +715,798 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1983</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1984</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1988</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1986</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1984</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1989</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1984</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1988</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1985</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1988</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1989</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1987</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1990</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1987</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1987</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1986</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>1989</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1987</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1986</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>1987</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>1991</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1988</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1989</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1987</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>1987</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>1984</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>1986</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1987</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>1985</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>1989</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>1990</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>1986</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>1987</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>1990</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>1991</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>1988</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>1986</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>1987</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>91</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>1988</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>1988</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42">
+        <v>1988</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
         <v>1984</v>
       </c>
-      <c r="C42" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43">
-        <v>1987</v>
-      </c>
       <c r="C43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>1987</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>1988</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47">
+        <v>1988</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
         <v>1987</v>
       </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48">
-        <v>1989</v>
-      </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>1989</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>1986</v>
+        <v>1989</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>1984</v>
+        <v>1987</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>1989</v>
+        <v>1984</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>1987</v>
+        <v>1990</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B57">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>1988</v>
+        <v>1990</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B59">
-        <v>1986</v>
+        <v>1988</v>
       </c>
       <c r="C59" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="C60" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>1989</v>
       </c>
       <c r="C61" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>1989</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B63">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="C63" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B64">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B65">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="C65" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B66">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B67">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B68">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>1988</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B70">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>1984</v>
       </c>
       <c r="C71" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72">
+        <v>1984</v>
+      </c>
+      <c r="C72" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D39" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>